<commit_message>
Delete cells that shouldn't be read in from workbook
</commit_message>
<xml_diff>
--- a/tests/bin/COUNTER_workbooks_for_tests/3_2019.xlsx
+++ b/tests/bin/COUNTER_workbooks_for_tests/3_2019.xlsx
@@ -2539,10 +2539,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG14"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2550,11 +2550,10 @@
     <col min="1" max="2" width="36" style="7" customWidth="1"/>
     <col min="3" max="10" width="10.7109375" style="7" customWidth="1"/>
     <col min="11" max="21" width="5.42578125" style="7" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" style="7" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="7"/>
+    <col min="22" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>56</v>
       </c>
@@ -2562,37 +2561,37 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>4</v>
       </c>
@@ -2657,7 +2656,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>29</v>
       </c>
@@ -2712,7 +2711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>29</v>
       </c>
@@ -2767,7 +2766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
@@ -2829,20 +2828,8 @@
       <c r="U11" s="8">
         <v>0</v>
       </c>
-      <c r="V11"/>
-      <c r="W11"/>
-      <c r="X11"/>
-      <c r="Y11"/>
-      <c r="Z11"/>
-      <c r="AA11"/>
-      <c r="AB11"/>
-      <c r="AC11"/>
-      <c r="AD11"/>
-      <c r="AE11"/>
-      <c r="AF11"/>
-      <c r="AG11"/>
-    </row>
-    <row r="12" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
@@ -2904,20 +2891,8 @@
       <c r="U12" s="8">
         <v>0</v>
       </c>
-      <c r="V12"/>
-      <c r="W12"/>
-      <c r="X12"/>
-      <c r="Y12"/>
-      <c r="Z12"/>
-      <c r="AA12"/>
-      <c r="AB12"/>
-      <c r="AC12"/>
-      <c r="AD12"/>
-      <c r="AE12"/>
-      <c r="AF12"/>
-      <c r="AG12"/>
-    </row>
-    <row r="13" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -2979,20 +2954,8 @@
       <c r="U13" s="8">
         <v>0</v>
       </c>
-      <c r="V13"/>
-      <c r="W13"/>
-      <c r="X13"/>
-      <c r="Y13"/>
-      <c r="Z13"/>
-      <c r="AA13"/>
-      <c r="AB13"/>
-      <c r="AC13"/>
-      <c r="AD13"/>
-      <c r="AE13"/>
-      <c r="AF13"/>
-      <c r="AG13"/>
-    </row>
-    <row r="14" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -3054,18 +3017,6 @@
       <c r="U14" s="8">
         <v>0</v>
       </c>
-      <c r="V14"/>
-      <c r="W14"/>
-      <c r="X14"/>
-      <c r="Y14"/>
-      <c r="Z14"/>
-      <c r="AA14"/>
-      <c r="AB14"/>
-      <c r="AC14"/>
-      <c r="AD14"/>
-      <c r="AE14"/>
-      <c r="AF14"/>
-      <c r="AG14"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
@@ -3075,61 +3026,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Self_Registration_Enabled xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
-    <AppVersion xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
-    <Invited_Teachers xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
-    <Templates xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
-    <NotebookType xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
-    <Teachers xmlns="c0ea4c96-c916-4356-b97d-707632d919c2">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <Students xmlns="c0ea4c96-c916-4356-b97d-707632d919c2">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <Student_Groups xmlns="c0ea4c96-c916-4356-b97d-707632d919c2">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <DefaultSectionNames xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
-    <Owner xmlns="c0ea4c96-c916-4356-b97d-707632d919c2">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Invited_Students xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
-    <FolderType xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
-    <CultureName xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008C8E71F4C809694A8FE86E6AAA0E1148" ma:contentTypeVersion="27" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="538bdd8bd283fda01d62e48cde48a5ac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="631de70e-6607-43af-ba40-c3d3dc8be270" xmlns:ns4="c0ea4c96-c916-4356-b97d-707632d919c2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c7a64bf384ce539eb83742694d227d69" ns3:_="" ns4:_="">
     <xsd:import namespace="631de70e-6607-43af-ba40-c3d3dc8be270"/>
@@ -3500,32 +3396,62 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82FCA75-9C69-4ADC-815D-0F0B7F6BE8D6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="c0ea4c96-c916-4356-b97d-707632d919c2"/>
-    <ds:schemaRef ds:uri="631de70e-6607-43af-ba40-c3d3dc8be270"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F7AE534-56F5-4478-AD1D-283DB00623BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Self_Registration_Enabled xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
+    <AppVersion xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
+    <Invited_Teachers xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
+    <Templates xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
+    <NotebookType xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
+    <Teachers xmlns="c0ea4c96-c916-4356-b97d-707632d919c2">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <Students xmlns="c0ea4c96-c916-4356-b97d-707632d919c2">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <Student_Groups xmlns="c0ea4c96-c916-4356-b97d-707632d919c2">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <DefaultSectionNames xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
+    <Owner xmlns="c0ea4c96-c916-4356-b97d-707632d919c2">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Invited_Students xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
+    <FolderType xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
+    <CultureName xmlns="c0ea4c96-c916-4356-b97d-707632d919c2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2D81E7E-A701-461B-982D-373F6BAC1D0F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3542,4 +3468,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F7AE534-56F5-4478-AD1D-283DB00623BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82FCA75-9C69-4ADC-815D-0F0B7F6BE8D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="c0ea4c96-c916-4356-b97d-707632d919c2"/>
+    <ds:schemaRef ds:uri="631de70e-6607-43af-ba40-c3d3dc8be270"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>